<commit_message>
Refactor scraper architecture; implement TCGPlayerClient, card parsing, and sealed price fetching; enhance Excel export functionality
</commit_message>
<xml_diff>
--- a/excelDocs/paldeanFates/pokemon_data.xlsx
+++ b/excelDocs/paldeanFates/pokemon_data.xlsx
@@ -717,7 +717,7 @@
         <v>472</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>1.68</v>
+        <v>1.75</v>
       </c>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3">
@@ -733,16 +733,16 @@
         <v/>
       </c>
       <c r="I2" s="3" t="n">
-        <v>15.67</v>
+        <v>14.49</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>61.18</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>79.42</v>
+        <v>92.26000000000001</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>9.869999999999999</v>
+        <v>7.34</v>
       </c>
       <c r="M2" s="3" t="n"/>
       <c r="N2" s="3" t="n"/>
@@ -789,7 +789,7 @@
         <v>472</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>5.74</v>
+        <v>5.62</v>
       </c>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3">
@@ -848,7 +848,7 @@
         <v>155</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>3.5</v>
+        <v>3.72</v>
       </c>
       <c r="E4" s="3" t="inlineStr"/>
       <c r="F4" s="3">
@@ -910,7 +910,7 @@
         <v>0.1</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F5" s="3">
         <f>IF(B5="common", 4, IF(B5="uncommon", 3, IF(B5="rare", 0.73878, 1)))</f>
@@ -968,7 +968,7 @@
         <v>472</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>2.76</v>
+        <v>3.3</v>
       </c>
       <c r="E6" s="3" t="inlineStr"/>
       <c r="F6" s="3">
@@ -1027,7 +1027,7 @@
         <v>472</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>1.74</v>
+        <v>1.85</v>
       </c>
       <c r="E7" s="3" t="inlineStr"/>
       <c r="F7" s="3">
@@ -1086,7 +1086,7 @@
         <v>472</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>3.34</v>
+        <v>3.26</v>
       </c>
       <c r="E8" s="3" t="inlineStr"/>
       <c r="F8" s="3">
@@ -1145,10 +1145,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="F9" s="3">
         <f>IF(B9="common", 4, IF(B9="uncommon", 3, IF(B9="rare", 0.73878, 1)))</f>
@@ -1206,7 +1206,7 @@
         <v>472</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>4.45</v>
+        <v>4.61</v>
       </c>
       <c r="E10" s="3" t="inlineStr"/>
       <c r="F10" s="3">
@@ -1265,10 +1265,10 @@
         <v>25</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0.29</v>
+        <v>0.32</v>
       </c>
       <c r="F11" s="3">
         <f>IF(B11="common", 4, IF(B11="uncommon", 3, IF(B11="rare", 0.73878, 1)))</f>
@@ -1326,7 +1326,7 @@
         <v>465</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>15.57</v>
+        <v>13.97</v>
       </c>
       <c r="E12" s="3" t="inlineStr"/>
       <c r="F12" s="3">
@@ -1390,7 +1390,7 @@
         <v>0.04</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F13" s="3">
         <f>IF(B13="common", 4, IF(B13="uncommon", 3, IF(B13="rare", 0.73878, 1)))</f>
@@ -1450,10 +1450,10 @@
         <v>40</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F14" s="3">
         <f>IF(B14="common", 4, IF(B14="uncommon", 3, IF(B14="rare", 0.73878, 1)))</f>
@@ -1508,7 +1508,7 @@
         <v>472</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>3.72</v>
+        <v>3.44</v>
       </c>
       <c r="E15" s="3" t="inlineStr"/>
       <c r="F15" s="3">
@@ -1564,7 +1564,7 @@
         <v>472</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>2.04</v>
+        <v>2.59</v>
       </c>
       <c r="E16" s="3" t="inlineStr"/>
       <c r="F16" s="3">
@@ -1620,10 +1620,10 @@
         <v>25</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0.2</v>
+        <v>0.14</v>
       </c>
       <c r="F17" s="3">
         <f>IF(B17="common", 4, IF(B17="uncommon", 3, IF(B17="rare", 0.73878, 1)))</f>
@@ -1681,7 +1681,7 @@
         <v>472</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>1.96</v>
+        <v>2.16</v>
       </c>
       <c r="E18" s="3" t="inlineStr"/>
       <c r="F18" s="3">
@@ -1737,10 +1737,10 @@
         <v>16</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>0.13</v>
+        <v>0.19</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="F19" s="3">
         <f>IF(B19="common", 4, IF(B19="uncommon", 3, IF(B19="rare", 0.73878, 1)))</f>
@@ -1795,7 +1795,7 @@
         <v>472</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>6.64</v>
+        <v>6.04</v>
       </c>
       <c r="E20" s="3" t="inlineStr"/>
       <c r="F20" s="3">
@@ -1851,10 +1851,10 @@
         <v>40</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="F21" s="3">
         <f>IF(B21="common", 4, IF(B21="uncommon", 3, IF(B21="rare", 0.73878, 1)))</f>
@@ -1912,7 +1912,7 @@
         <v>472</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>5.3</v>
+        <v>5.52</v>
       </c>
       <c r="E22" s="3" t="inlineStr"/>
       <c r="F22" s="3">
@@ -1971,7 +1971,7 @@
         <v>63</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>3.76</v>
+        <v>3.74</v>
       </c>
       <c r="E23" s="3" t="inlineStr"/>
       <c r="F23" s="3">
@@ -2030,7 +2030,7 @@
         <v>465</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>304.36</v>
+        <v>268.34</v>
       </c>
       <c r="E24" s="3" t="inlineStr"/>
       <c r="F24" s="3">
@@ -2086,10 +2086,10 @@
         <v>40</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>0.23</v>
+        <v>0.26</v>
       </c>
       <c r="F25" s="3">
         <f>IF(B25="common", 4, IF(B25="uncommon", 3, IF(B25="rare", 0.73878, 1)))</f>
@@ -2144,7 +2144,7 @@
         <v>472</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>21.36</v>
+        <v>23.18</v>
       </c>
       <c r="E26" s="3" t="inlineStr"/>
       <c r="F26" s="3">
@@ -2200,10 +2200,10 @@
         <v>25</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>0.25</v>
+        <v>0.28</v>
       </c>
       <c r="F27" s="3">
         <f>IF(B27="common", 4, IF(B27="uncommon", 3, IF(B27="rare", 0.73878, 1)))</f>
@@ -2258,7 +2258,7 @@
         <v>472</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>13.66</v>
+        <v>12.18</v>
       </c>
       <c r="E28" s="3" t="inlineStr"/>
       <c r="F28" s="3">
@@ -2314,7 +2314,7 @@
         <v>372</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>6.7</v>
+        <v>7.28</v>
       </c>
       <c r="E29" s="3" t="inlineStr"/>
       <c r="F29" s="3">
@@ -2370,7 +2370,7 @@
         <v>372</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>7.28</v>
+        <v>6.12</v>
       </c>
       <c r="E30" s="3" t="inlineStr"/>
       <c r="F30" s="3">
@@ -2429,7 +2429,7 @@
         <v>0.06</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="F31" s="3">
         <f>IF(B31="common", 4, IF(B31="uncommon", 3, IF(B31="rare", 0.73878, 1)))</f>
@@ -2484,10 +2484,10 @@
         <v>40</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
       <c r="F32" s="3">
         <f>IF(B32="common", 4, IF(B32="uncommon", 3, IF(B32="rare", 0.73878, 1)))</f>
@@ -2542,7 +2542,7 @@
         <v>472</v>
       </c>
       <c r="D33" s="3" t="n">
-        <v>3.29</v>
+        <v>3.25</v>
       </c>
       <c r="E33" s="3" t="inlineStr"/>
       <c r="F33" s="3">
@@ -2601,7 +2601,7 @@
         <v>0.04</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>0.16</v>
+        <v>0.11</v>
       </c>
       <c r="F34" s="3">
         <f>IF(B34="common", 4, IF(B34="uncommon", 3, IF(B34="rare", 0.73878, 1)))</f>
@@ -2712,7 +2712,7 @@
         <v>465</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>16.54</v>
+        <v>17.21</v>
       </c>
       <c r="E36" s="3" t="inlineStr"/>
       <c r="F36" s="3">
@@ -2768,10 +2768,10 @@
         <v>40</v>
       </c>
       <c r="D37" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="F37" s="3">
         <f>IF(B37="common", 4, IF(B37="uncommon", 3, IF(B37="rare", 0.73878, 1)))</f>
@@ -2826,10 +2826,10 @@
         <v>40</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E38" s="3" t="n">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="F38" s="3">
         <f>IF(B38="common", 4, IF(B38="uncommon", 3, IF(B38="rare", 0.73878, 1)))</f>
@@ -2884,10 +2884,10 @@
         <v>16</v>
       </c>
       <c r="D39" s="3" t="n">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>0.13</v>
+        <v>0.17</v>
       </c>
       <c r="F39" s="3">
         <f>IF(B39="common", 4, IF(B39="uncommon", 3, IF(B39="rare", 0.73878, 1)))</f>
@@ -2942,7 +2942,7 @@
         <v>472</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>1.75</v>
+        <v>1.84</v>
       </c>
       <c r="E40" s="3" t="inlineStr"/>
       <c r="F40" s="3">
@@ -3001,7 +3001,7 @@
         <v>0.08</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="F41" s="3">
         <f>IF(B41="common", 4, IF(B41="uncommon", 3, IF(B41="rare", 0.73878, 1)))</f>
@@ -3056,7 +3056,7 @@
         <v>472</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>4.93</v>
+        <v>4.6</v>
       </c>
       <c r="E42" s="3" t="inlineStr"/>
       <c r="F42" s="3">
@@ -3112,10 +3112,10 @@
         <v>40</v>
       </c>
       <c r="D43" s="3" t="n">
-        <v>0.05</v>
+        <v>0.09</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="F43" s="3">
         <f>IF(B43="common", 4, IF(B43="uncommon", 3, IF(B43="rare", 0.73878, 1)))</f>
@@ -3170,7 +3170,7 @@
         <v>472</v>
       </c>
       <c r="D44" s="3" t="n">
-        <v>20.45</v>
+        <v>19.35</v>
       </c>
       <c r="E44" s="3" t="inlineStr"/>
       <c r="F44" s="3">
@@ -3226,7 +3226,7 @@
         <v>472</v>
       </c>
       <c r="D45" s="3" t="n">
-        <v>2.59</v>
+        <v>3.12</v>
       </c>
       <c r="E45" s="3" t="inlineStr"/>
       <c r="F45" s="3">
@@ -3282,7 +3282,7 @@
         <v>472</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>3.11</v>
+        <v>3.13</v>
       </c>
       <c r="E46" s="3" t="inlineStr"/>
       <c r="F46" s="3">
@@ -3338,7 +3338,7 @@
         <v>472</v>
       </c>
       <c r="D47" s="3" t="n">
-        <v>2.3</v>
+        <v>2.4</v>
       </c>
       <c r="E47" s="3" t="inlineStr"/>
       <c r="F47" s="3">
@@ -3394,7 +3394,7 @@
         <v>472</v>
       </c>
       <c r="D48" s="3" t="n">
-        <v>2.35</v>
+        <v>2.48</v>
       </c>
       <c r="E48" s="3" t="inlineStr"/>
       <c r="F48" s="3">
@@ -3450,10 +3450,10 @@
         <v>25</v>
       </c>
       <c r="D49" s="3" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="F49" s="3">
         <f>IF(B49="common", 4, IF(B49="uncommon", 3, IF(B49="rare", 0.73878, 1)))</f>
@@ -3508,7 +3508,7 @@
         <v>472</v>
       </c>
       <c r="D50" s="3" t="n">
-        <v>2.04</v>
+        <v>2.13</v>
       </c>
       <c r="E50" s="3" t="inlineStr"/>
       <c r="F50" s="3">
@@ -3564,7 +3564,7 @@
         <v>472</v>
       </c>
       <c r="D51" s="3" t="n">
-        <v>6.34</v>
+        <v>5.85</v>
       </c>
       <c r="E51" s="3" t="inlineStr"/>
       <c r="F51" s="3">
@@ -3620,10 +3620,10 @@
         <v>25</v>
       </c>
       <c r="D52" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="F52" s="3">
         <f>IF(B52="common", 4, IF(B52="uncommon", 3, IF(B52="rare", 0.73878, 1)))</f>
@@ -3678,7 +3678,7 @@
         <v>472</v>
       </c>
       <c r="D53" s="3" t="n">
-        <v>3.06</v>
+        <v>2.92</v>
       </c>
       <c r="E53" s="3" t="inlineStr"/>
       <c r="F53" s="3">
@@ -3734,7 +3734,7 @@
         <v>472</v>
       </c>
       <c r="D54" s="3" t="n">
-        <v>9.27</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="E54" s="3" t="inlineStr"/>
       <c r="F54" s="3">
@@ -3790,7 +3790,7 @@
         <v>63</v>
       </c>
       <c r="D55" s="3" t="n">
-        <v>0.44</v>
+        <v>0.51</v>
       </c>
       <c r="E55" s="3" t="inlineStr"/>
       <c r="F55" s="3">
@@ -3846,7 +3846,7 @@
         <v>155</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>1.07</v>
+        <v>1.13</v>
       </c>
       <c r="E56" s="3" t="inlineStr"/>
       <c r="F56" s="3">
@@ -3902,10 +3902,10 @@
         <v>40</v>
       </c>
       <c r="D57" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F57" s="3">
         <f>IF(B57="common", 4, IF(B57="uncommon", 3, IF(B57="rare", 0.73878, 1)))</f>
@@ -4018,10 +4018,10 @@
         <v>40</v>
       </c>
       <c r="D59" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F59" s="3">
         <f>IF(B59="common", 4, IF(B59="uncommon", 3, IF(B59="rare", 0.73878, 1)))</f>
@@ -4076,7 +4076,7 @@
         <v>472</v>
       </c>
       <c r="D60" s="3" t="n">
-        <v>3.54</v>
+        <v>3.71</v>
       </c>
       <c r="E60" s="3" t="inlineStr"/>
       <c r="F60" s="3">
@@ -4132,7 +4132,7 @@
         <v>472</v>
       </c>
       <c r="D61" s="3" t="n">
-        <v>2.67</v>
+        <v>2.97</v>
       </c>
       <c r="E61" s="3" t="inlineStr"/>
       <c r="F61" s="3">
@@ -4188,10 +4188,10 @@
         <v>40</v>
       </c>
       <c r="D62" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E62" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F62" s="3">
         <f>IF(B62="common", 4, IF(B62="uncommon", 3, IF(B62="rare", 0.73878, 1)))</f>
@@ -4246,7 +4246,7 @@
         <v>472</v>
       </c>
       <c r="D63" s="3" t="n">
-        <v>1.72</v>
+        <v>1.63</v>
       </c>
       <c r="E63" s="3" t="inlineStr"/>
       <c r="F63" s="3">
@@ -4302,7 +4302,7 @@
         <v>63</v>
       </c>
       <c r="D64" s="3" t="n">
-        <v>0.43</v>
+        <v>0.51</v>
       </c>
       <c r="E64" s="3" t="inlineStr"/>
       <c r="F64" s="3">
@@ -4358,7 +4358,7 @@
         <v>155</v>
       </c>
       <c r="D65" s="3" t="n">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="E65" s="3" t="inlineStr"/>
       <c r="F65" s="3">
@@ -4414,10 +4414,10 @@
         <v>40</v>
       </c>
       <c r="D66" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="F66" s="3">
         <f>IF(B66="common", 4, IF(B66="uncommon", 3, IF(B66="rare", 0.73878, 1)))</f>
@@ -4472,7 +4472,7 @@
         <v>472</v>
       </c>
       <c r="D67" s="3" t="n">
-        <v>3.62</v>
+        <v>2.97</v>
       </c>
       <c r="E67" s="3" t="inlineStr"/>
       <c r="F67" s="3">
@@ -4528,7 +4528,7 @@
         <v>63</v>
       </c>
       <c r="D68" s="3" t="n">
-        <v>0.77</v>
+        <v>0.86</v>
       </c>
       <c r="E68" s="3" t="inlineStr"/>
       <c r="F68" s="3">
@@ -4584,7 +4584,7 @@
         <v>155</v>
       </c>
       <c r="D69" s="3" t="n">
-        <v>13.11</v>
+        <v>5.88</v>
       </c>
       <c r="E69" s="3" t="inlineStr"/>
       <c r="F69" s="3">
@@ -4640,7 +4640,7 @@
         <v>465</v>
       </c>
       <c r="D70" s="3" t="n">
-        <v>140.61</v>
+        <v>125.23</v>
       </c>
       <c r="E70" s="3" t="inlineStr"/>
       <c r="F70" s="3">
@@ -4696,7 +4696,7 @@
         <v>472</v>
       </c>
       <c r="D71" s="3" t="n">
-        <v>1.62</v>
+        <v>1.8</v>
       </c>
       <c r="E71" s="3" t="inlineStr"/>
       <c r="F71" s="3">
@@ -4755,7 +4755,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E72" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F72" s="3">
         <f>IF(B72="common", 4, IF(B72="uncommon", 3, IF(B72="rare", 0.73878, 1)))</f>
@@ -4810,10 +4810,10 @@
         <v>25</v>
       </c>
       <c r="D73" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="E73" s="3" t="n">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="F73" s="3">
         <f>IF(B73="common", 4, IF(B73="uncommon", 3, IF(B73="rare", 0.73878, 1)))</f>
@@ -4868,7 +4868,7 @@
         <v>16</v>
       </c>
       <c r="D74" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E74" s="3" t="n">
         <v>0.15</v>
@@ -4926,10 +4926,10 @@
         <v>40</v>
       </c>
       <c r="D75" s="3" t="n">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E75" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F75" s="3">
         <f>IF(B75="common", 4, IF(B75="uncommon", 3, IF(B75="rare", 0.73878, 1)))</f>
@@ -4984,7 +4984,7 @@
         <v>472</v>
       </c>
       <c r="D76" s="3" t="n">
-        <v>1.98</v>
+        <v>1.92</v>
       </c>
       <c r="E76" s="3" t="inlineStr"/>
       <c r="F76" s="3">
@@ -5040,7 +5040,7 @@
         <v>155</v>
       </c>
       <c r="D77" s="3" t="n">
-        <v>0.79</v>
+        <v>0.92</v>
       </c>
       <c r="E77" s="3" t="inlineStr"/>
       <c r="F77" s="3">
@@ -5096,7 +5096,7 @@
         <v>472</v>
       </c>
       <c r="D78" s="3" t="n">
-        <v>3.35</v>
+        <v>3.47</v>
       </c>
       <c r="E78" s="3" t="inlineStr"/>
       <c r="F78" s="3">
@@ -5152,7 +5152,7 @@
         <v>472</v>
       </c>
       <c r="D79" s="3" t="n">
-        <v>1.6</v>
+        <v>1.67</v>
       </c>
       <c r="E79" s="3" t="inlineStr"/>
       <c r="F79" s="3">
@@ -5208,10 +5208,10 @@
         <v>25</v>
       </c>
       <c r="D80" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F80" s="3">
         <f>IF(B80="common", 4, IF(B80="uncommon", 3, IF(B80="rare", 0.73878, 1)))</f>
@@ -5266,7 +5266,7 @@
         <v>63</v>
       </c>
       <c r="D81" s="3" t="n">
-        <v>0.54</v>
+        <v>0.61</v>
       </c>
       <c r="E81" s="3" t="inlineStr"/>
       <c r="F81" s="3">
@@ -5322,10 +5322,10 @@
         <v>40</v>
       </c>
       <c r="D82" s="3" t="n">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="E82" s="3" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="F82" s="3">
         <f>IF(B82="common", 4, IF(B82="uncommon", 3, IF(B82="rare", 0.73878, 1)))</f>
@@ -5380,7 +5380,7 @@
         <v>472</v>
       </c>
       <c r="D83" s="3" t="n">
-        <v>1.73</v>
+        <v>1.71</v>
       </c>
       <c r="E83" s="3" t="inlineStr"/>
       <c r="F83" s="3">
@@ -5439,7 +5439,7 @@
         <v>0.11</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="F84" s="3">
         <f>IF(B84="common", 4, IF(B84="uncommon", 3, IF(B84="rare", 0.73878, 1)))</f>
@@ -5494,7 +5494,7 @@
         <v>472</v>
       </c>
       <c r="D85" s="3" t="n">
-        <v>9.210000000000001</v>
+        <v>8.19</v>
       </c>
       <c r="E85" s="3" t="inlineStr"/>
       <c r="F85" s="3">
@@ -5550,7 +5550,7 @@
         <v>16</v>
       </c>
       <c r="D86" s="3" t="n">
-        <v>0.11</v>
+        <v>0.21</v>
       </c>
       <c r="E86" s="3" t="n">
         <v>0.17</v>
@@ -5608,7 +5608,7 @@
         <v>472</v>
       </c>
       <c r="D87" s="3" t="n">
-        <v>2.43</v>
+        <v>2.35</v>
       </c>
       <c r="E87" s="3" t="inlineStr"/>
       <c r="F87" s="3">
@@ -5664,10 +5664,10 @@
         <v>16</v>
       </c>
       <c r="D88" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E88" s="3" t="n">
-        <v>0.17</v>
+        <v>0.13</v>
       </c>
       <c r="F88" s="3">
         <f>IF(B88="common", 4, IF(B88="uncommon", 3, IF(B88="rare", 0.73878, 1)))</f>
@@ -5722,7 +5722,7 @@
         <v>472</v>
       </c>
       <c r="D89" s="3" t="n">
-        <v>1.55</v>
+        <v>1.51</v>
       </c>
       <c r="E89" s="3" t="inlineStr"/>
       <c r="F89" s="3">
@@ -5778,10 +5778,10 @@
         <v>25</v>
       </c>
       <c r="D90" s="3" t="n">
-        <v>0.3</v>
+        <v>0.21</v>
       </c>
       <c r="E90" s="3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.74</v>
       </c>
       <c r="F90" s="3">
         <f>IF(B90="common", 4, IF(B90="uncommon", 3, IF(B90="rare", 0.73878, 1)))</f>
@@ -5836,7 +5836,7 @@
         <v>465</v>
       </c>
       <c r="D91" s="3" t="n">
-        <v>28.12</v>
+        <v>26.59</v>
       </c>
       <c r="E91" s="3" t="inlineStr"/>
       <c r="F91" s="3">
@@ -5892,7 +5892,7 @@
         <v>63</v>
       </c>
       <c r="D92" s="3" t="n">
-        <v>0.52</v>
+        <v>0.62</v>
       </c>
       <c r="E92" s="3" t="inlineStr"/>
       <c r="F92" s="3">
@@ -5948,7 +5948,7 @@
         <v>472</v>
       </c>
       <c r="D93" s="3" t="n">
-        <v>6.3</v>
+        <v>6.6</v>
       </c>
       <c r="E93" s="3" t="inlineStr"/>
       <c r="F93" s="3">
@@ -6004,7 +6004,7 @@
         <v>76</v>
       </c>
       <c r="D94" s="3" t="n">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="E94" s="3" t="inlineStr"/>
       <c r="F94" s="3">
@@ -6060,7 +6060,7 @@
         <v>472</v>
       </c>
       <c r="D95" s="3" t="n">
-        <v>2.79</v>
+        <v>2.61</v>
       </c>
       <c r="E95" s="3" t="inlineStr"/>
       <c r="F95" s="3">
@@ -6116,7 +6116,7 @@
         <v>472</v>
       </c>
       <c r="D96" s="3" t="n">
-        <v>5.27</v>
+        <v>4.49</v>
       </c>
       <c r="E96" s="3" t="inlineStr"/>
       <c r="F96" s="3">
@@ -6172,10 +6172,10 @@
         <v>25</v>
       </c>
       <c r="D97" s="3" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="F97" s="3">
         <f>IF(B97="common", 4, IF(B97="uncommon", 3, IF(B97="rare", 0.73878, 1)))</f>
@@ -6230,7 +6230,7 @@
         <v>472</v>
       </c>
       <c r="D98" s="3" t="n">
-        <v>1.64</v>
+        <v>1.92</v>
       </c>
       <c r="E98" s="3" t="inlineStr"/>
       <c r="F98" s="3">
@@ -6286,7 +6286,7 @@
         <v>472</v>
       </c>
       <c r="D99" s="3" t="n">
-        <v>2.7</v>
+        <v>2.89</v>
       </c>
       <c r="E99" s="3" t="inlineStr"/>
       <c r="F99" s="3">
@@ -6342,10 +6342,10 @@
         <v>25</v>
       </c>
       <c r="D100" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E100" s="3" t="n">
-        <v>0.29</v>
+        <v>0.2</v>
       </c>
       <c r="F100" s="3">
         <f>IF(B100="common", 4, IF(B100="uncommon", 3, IF(B100="rare", 0.73878, 1)))</f>
@@ -6400,7 +6400,7 @@
         <v>472</v>
       </c>
       <c r="D101" s="3" t="n">
-        <v>10.45</v>
+        <v>6.58</v>
       </c>
       <c r="E101" s="3" t="inlineStr"/>
       <c r="F101" s="3">
@@ -6456,7 +6456,7 @@
         <v>472</v>
       </c>
       <c r="D102" s="3" t="n">
-        <v>3.7</v>
+        <v>4.45</v>
       </c>
       <c r="E102" s="3" t="inlineStr"/>
       <c r="F102" s="3">
@@ -6512,7 +6512,7 @@
         <v>372</v>
       </c>
       <c r="D103" s="3" t="n">
-        <v>9.23</v>
+        <v>10.07</v>
       </c>
       <c r="E103" s="3" t="inlineStr"/>
       <c r="F103" s="3">
@@ -6568,10 +6568,10 @@
         <v>25</v>
       </c>
       <c r="D104" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E104" s="3" t="n">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="F104" s="3">
         <f>IF(B104="common", 4, IF(B104="uncommon", 3, IF(B104="rare", 0.73878, 1)))</f>
@@ -6626,7 +6626,7 @@
         <v>40</v>
       </c>
       <c r="D105" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E105" s="3" t="n">
         <v>0.14</v>
@@ -6687,7 +6687,7 @@
         <v>0.05</v>
       </c>
       <c r="E106" s="3" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F106" s="3">
         <f>IF(B106="common", 4, IF(B106="uncommon", 3, IF(B106="rare", 0.73878, 1)))</f>
@@ -6742,7 +6742,7 @@
         <v>472</v>
       </c>
       <c r="D107" s="3" t="n">
-        <v>5.35</v>
+        <v>4.72</v>
       </c>
       <c r="E107" s="3" t="inlineStr"/>
       <c r="F107" s="3">
@@ -6798,7 +6798,7 @@
         <v>472</v>
       </c>
       <c r="D108" s="3" t="n">
-        <v>13.03</v>
+        <v>15.75</v>
       </c>
       <c r="E108" s="3" t="inlineStr"/>
       <c r="F108" s="3">
@@ -6854,7 +6854,7 @@
         <v>472</v>
       </c>
       <c r="D109" s="3" t="n">
-        <v>4.28</v>
+        <v>3.9</v>
       </c>
       <c r="E109" s="3" t="inlineStr"/>
       <c r="F109" s="3">
@@ -6910,7 +6910,7 @@
         <v>472</v>
       </c>
       <c r="D110" s="3" t="n">
-        <v>8.210000000000001</v>
+        <v>7.71</v>
       </c>
       <c r="E110" s="3" t="inlineStr"/>
       <c r="F110" s="3">
@@ -6966,10 +6966,10 @@
         <v>16</v>
       </c>
       <c r="D111" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E111" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="F111" s="3">
         <f>IF(B111="common", 4, IF(B111="uncommon", 3, IF(B111="rare", 0.73878, 1)))</f>
@@ -7024,7 +7024,7 @@
         <v>472</v>
       </c>
       <c r="D112" s="3" t="n">
-        <v>1.79</v>
+        <v>1.57</v>
       </c>
       <c r="E112" s="3" t="inlineStr"/>
       <c r="F112" s="3">
@@ -7080,10 +7080,10 @@
         <v>40</v>
       </c>
       <c r="D113" s="3" t="n">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="E113" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F113" s="3">
         <f>IF(B113="common", 4, IF(B113="uncommon", 3, IF(B113="rare", 0.73878, 1)))</f>
@@ -7138,10 +7138,10 @@
         <v>16</v>
       </c>
       <c r="D114" s="3" t="n">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="E114" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F114" s="3">
         <f>IF(B114="common", 4, IF(B114="uncommon", 3, IF(B114="rare", 0.73878, 1)))</f>
@@ -7196,10 +7196,10 @@
         <v>40</v>
       </c>
       <c r="D115" s="3" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E115" s="3" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="F115" s="3">
         <f>IF(B115="common", 4, IF(B115="uncommon", 3, IF(B115="rare", 0.73878, 1)))</f>
@@ -7254,7 +7254,7 @@
         <v>472</v>
       </c>
       <c r="D116" s="3" t="n">
-        <v>2.87</v>
+        <v>3.23</v>
       </c>
       <c r="E116" s="3" t="inlineStr"/>
       <c r="F116" s="3">
@@ -7310,10 +7310,10 @@
         <v>40</v>
       </c>
       <c r="D117" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E117" s="3" t="n">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="F117" s="3">
         <f>IF(B117="common", 4, IF(B117="uncommon", 3, IF(B117="rare", 0.73878, 1)))</f>
@@ -7368,10 +7368,10 @@
         <v>40</v>
       </c>
       <c r="D118" s="3" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="E118" s="3" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="F118" s="3">
         <f>IF(B118="common", 4, IF(B118="uncommon", 3, IF(B118="rare", 0.73878, 1)))</f>
@@ -7426,10 +7426,10 @@
         <v>25</v>
       </c>
       <c r="D119" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E119" s="3" t="n">
-        <v>0.18</v>
+        <v>0.23</v>
       </c>
       <c r="F119" s="3">
         <f>IF(B119="common", 4, IF(B119="uncommon", 3, IF(B119="rare", 0.73878, 1)))</f>
@@ -7484,7 +7484,7 @@
         <v>472</v>
       </c>
       <c r="D120" s="3" t="n">
-        <v>9.699999999999999</v>
+        <v>12</v>
       </c>
       <c r="E120" s="3" t="inlineStr"/>
       <c r="F120" s="3">
@@ -7540,7 +7540,7 @@
         <v>155</v>
       </c>
       <c r="D121" s="3" t="n">
-        <v>26.26</v>
+        <v>24.92</v>
       </c>
       <c r="E121" s="3" t="inlineStr"/>
       <c r="F121" s="3">
@@ -7596,7 +7596,7 @@
         <v>465</v>
       </c>
       <c r="D122" s="3" t="n">
-        <v>634.08</v>
+        <v>542.12</v>
       </c>
       <c r="E122" s="3" t="inlineStr"/>
       <c r="F122" s="3">
@@ -7652,7 +7652,7 @@
         <v>40</v>
       </c>
       <c r="D123" s="3" t="n">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="E123" s="3" t="n">
         <v>0.15</v>
@@ -7710,7 +7710,7 @@
         <v>472</v>
       </c>
       <c r="D124" s="3" t="n">
-        <v>2.47</v>
+        <v>2.42</v>
       </c>
       <c r="E124" s="3" t="inlineStr"/>
       <c r="F124" s="3">
@@ -7766,10 +7766,10 @@
         <v>16</v>
       </c>
       <c r="D125" s="3" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="E125" s="3" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
       <c r="F125" s="3">
         <f>IF(B125="common", 4, IF(B125="uncommon", 3, IF(B125="rare", 0.73878, 1)))</f>
@@ -7824,7 +7824,7 @@
         <v>472</v>
       </c>
       <c r="D126" s="3" t="n">
-        <v>16.1</v>
+        <v>18.64</v>
       </c>
       <c r="E126" s="3" t="inlineStr"/>
       <c r="F126" s="3">
@@ -7880,7 +7880,7 @@
         <v>372</v>
       </c>
       <c r="D127" s="3" t="n">
-        <v>10.52</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="E127" s="3" t="inlineStr"/>
       <c r="F127" s="3">
@@ -7936,10 +7936,10 @@
         <v>25</v>
       </c>
       <c r="D128" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E128" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F128" s="3">
         <f>IF(B128="common", 4, IF(B128="uncommon", 3, IF(B128="rare", 0.73878, 1)))</f>
@@ -7994,7 +7994,7 @@
         <v>472</v>
       </c>
       <c r="D129" s="3" t="n">
-        <v>3.17</v>
+        <v>2.88</v>
       </c>
       <c r="E129" s="3" t="inlineStr"/>
       <c r="F129" s="3">
@@ -8050,7 +8050,7 @@
         <v>472</v>
       </c>
       <c r="D130" s="3" t="n">
-        <v>1.69</v>
+        <v>1.75</v>
       </c>
       <c r="E130" s="3" t="inlineStr"/>
       <c r="F130" s="3">
@@ -8106,7 +8106,7 @@
         <v>472</v>
       </c>
       <c r="D131" s="3" t="n">
-        <v>1.98</v>
+        <v>2.13</v>
       </c>
       <c r="E131" s="3" t="inlineStr"/>
       <c r="F131" s="3">
@@ -8165,7 +8165,7 @@
         <v>0.08</v>
       </c>
       <c r="E132" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F132" s="3">
         <f>IF(B132="common", 4, IF(B132="uncommon", 3, IF(B132="rare", 0.73878, 1)))</f>
@@ -8220,7 +8220,7 @@
         <v>472</v>
       </c>
       <c r="D133" s="3" t="n">
-        <v>2.43</v>
+        <v>2.68</v>
       </c>
       <c r="E133" s="3" t="inlineStr"/>
       <c r="F133" s="3">
@@ -8279,7 +8279,7 @@
         <v>0.04</v>
       </c>
       <c r="E134" s="3" t="n">
-        <v>0.12</v>
+        <v>0.14</v>
       </c>
       <c r="F134" s="3">
         <f>IF(B134="common", 4, IF(B134="uncommon", 3, IF(B134="rare", 0.73878, 1)))</f>
@@ -8334,7 +8334,7 @@
         <v>76</v>
       </c>
       <c r="D135" s="3" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="E135" s="3" t="inlineStr"/>
       <c r="F135" s="3">
@@ -8390,7 +8390,7 @@
         <v>465</v>
       </c>
       <c r="D136" s="3" t="n">
-        <v>5.87</v>
+        <v>6.05</v>
       </c>
       <c r="E136" s="3" t="inlineStr"/>
       <c r="F136" s="3">
@@ -8446,10 +8446,10 @@
         <v>25</v>
       </c>
       <c r="D137" s="3" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E137" s="3" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="F137" s="3">
         <f>IF(B137="common", 4, IF(B137="uncommon", 3, IF(B137="rare", 0.73878, 1)))</f>
@@ -8504,10 +8504,10 @@
         <v>25</v>
       </c>
       <c r="D138" s="3" t="n">
-        <v>0.33</v>
+        <v>0.21</v>
       </c>
       <c r="E138" s="3" t="n">
-        <v>0.51</v>
+        <v>0.67</v>
       </c>
       <c r="F138" s="3">
         <f>IF(B138="common", 4, IF(B138="uncommon", 3, IF(B138="rare", 0.73878, 1)))</f>
@@ -8562,10 +8562,10 @@
         <v>40</v>
       </c>
       <c r="D139" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="F139" s="3">
         <f>IF(B139="common", 4, IF(B139="uncommon", 3, IF(B139="rare", 0.73878, 1)))</f>
@@ -8620,7 +8620,7 @@
         <v>472</v>
       </c>
       <c r="D140" s="3" t="n">
-        <v>3.32</v>
+        <v>3.83</v>
       </c>
       <c r="E140" s="3" t="inlineStr"/>
       <c r="F140" s="3">
@@ -8676,7 +8676,7 @@
         <v>63</v>
       </c>
       <c r="D141" s="3" t="n">
-        <v>0.43</v>
+        <v>0.59</v>
       </c>
       <c r="E141" s="3" t="inlineStr"/>
       <c r="F141" s="3">
@@ -8732,7 +8732,7 @@
         <v>155</v>
       </c>
       <c r="D142" s="3" t="n">
-        <v>1.99</v>
+        <v>1.59</v>
       </c>
       <c r="E142" s="3" t="inlineStr"/>
       <c r="F142" s="3">
@@ -8788,10 +8788,10 @@
         <v>40</v>
       </c>
       <c r="D143" s="3" t="n">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="E143" s="3" t="n">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
       <c r="F143" s="3">
         <f>IF(B143="common", 4, IF(B143="uncommon", 3, IF(B143="rare", 0.73878, 1)))</f>
@@ -8846,7 +8846,7 @@
         <v>472</v>
       </c>
       <c r="D144" s="3" t="n">
-        <v>5.23</v>
+        <v>5.96</v>
       </c>
       <c r="E144" s="3" t="inlineStr"/>
       <c r="F144" s="3">
@@ -8902,10 +8902,10 @@
         <v>25</v>
       </c>
       <c r="D145" s="3" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>0.09</v>
+        <v>0.17</v>
       </c>
       <c r="F145" s="3">
         <f>IF(B145="common", 4, IF(B145="uncommon", 3, IF(B145="rare", 0.73878, 1)))</f>
@@ -8960,7 +8960,7 @@
         <v>472</v>
       </c>
       <c r="D146" s="3" t="n">
-        <v>2.66</v>
+        <v>2.51</v>
       </c>
       <c r="E146" s="3" t="inlineStr"/>
       <c r="F146" s="3">
@@ -9016,7 +9016,7 @@
         <v>472</v>
       </c>
       <c r="D147" s="3" t="n">
-        <v>2.11</v>
+        <v>1.96</v>
       </c>
       <c r="E147" s="3" t="inlineStr"/>
       <c r="F147" s="3">
@@ -9072,7 +9072,7 @@
         <v>472</v>
       </c>
       <c r="D148" s="3" t="n">
-        <v>5.06</v>
+        <v>4.72</v>
       </c>
       <c r="E148" s="3" t="inlineStr"/>
       <c r="F148" s="3">
@@ -9128,7 +9128,7 @@
         <v>472</v>
       </c>
       <c r="D149" s="3" t="n">
-        <v>1.83</v>
+        <v>1.85</v>
       </c>
       <c r="E149" s="3" t="inlineStr"/>
       <c r="F149" s="3">
@@ -9184,7 +9184,7 @@
         <v>42</v>
       </c>
       <c r="D150" s="3" t="n">
-        <v>1.85</v>
+        <v>1.39</v>
       </c>
       <c r="E150" s="3" t="inlineStr"/>
       <c r="F150" s="3">
@@ -9240,7 +9240,7 @@
         <v>63</v>
       </c>
       <c r="D151" s="3" t="n">
-        <v>0.55</v>
+        <v>0.62</v>
       </c>
       <c r="E151" s="3" t="inlineStr"/>
       <c r="F151" s="3">
@@ -9352,7 +9352,7 @@
         <v>40</v>
       </c>
       <c r="D153" s="3" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="E153" s="3" t="n">
         <v>0.1</v>
@@ -9413,7 +9413,7 @@
         <v>0.03</v>
       </c>
       <c r="E154" s="3" t="n">
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="F154" s="3">
         <f>IF(B154="common", 4, IF(B154="uncommon", 3, IF(B154="rare", 0.73878, 1)))</f>
@@ -9468,7 +9468,7 @@
         <v>76</v>
       </c>
       <c r="D155" s="3" t="n">
-        <v>0.72</v>
+        <v>0.55</v>
       </c>
       <c r="E155" s="3" t="inlineStr"/>
       <c r="F155" s="3">
@@ -9524,7 +9524,7 @@
         <v>76</v>
       </c>
       <c r="D156" s="3" t="n">
-        <v>0.72</v>
+        <v>0.63</v>
       </c>
       <c r="E156" s="3" t="inlineStr"/>
       <c r="F156" s="3">
@@ -9580,7 +9580,7 @@
         <v>472</v>
       </c>
       <c r="D157" s="3" t="n">
-        <v>2.06</v>
+        <v>2.23</v>
       </c>
       <c r="E157" s="3" t="inlineStr"/>
       <c r="F157" s="3">
@@ -9636,7 +9636,7 @@
         <v>472</v>
       </c>
       <c r="D158" s="3" t="n">
-        <v>2.51</v>
+        <v>2.52</v>
       </c>
       <c r="E158" s="3" t="inlineStr"/>
       <c r="F158" s="3">
@@ -9692,7 +9692,7 @@
         <v>472</v>
       </c>
       <c r="D159" s="3" t="n">
-        <v>2.04</v>
+        <v>2.07</v>
       </c>
       <c r="E159" s="3" t="inlineStr"/>
       <c r="F159" s="3">
@@ -9748,10 +9748,10 @@
         <v>40</v>
       </c>
       <c r="D160" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E160" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F160" s="3">
         <f>IF(B160="common", 4, IF(B160="uncommon", 3, IF(B160="rare", 0.73878, 1)))</f>
@@ -9862,7 +9862,7 @@
         <v>472</v>
       </c>
       <c r="D162" s="3" t="n">
-        <v>2.76</v>
+        <v>2.75</v>
       </c>
       <c r="E162" s="3" t="inlineStr"/>
       <c r="F162" s="3">
@@ -9918,7 +9918,7 @@
         <v>42</v>
       </c>
       <c r="D163" s="3" t="n">
-        <v>1.97</v>
+        <v>1.26</v>
       </c>
       <c r="E163" s="3" t="inlineStr"/>
       <c r="F163" s="3">
@@ -9974,7 +9974,7 @@
         <v>472</v>
       </c>
       <c r="D164" s="3" t="n">
-        <v>2.83</v>
+        <v>2.87</v>
       </c>
       <c r="E164" s="3" t="inlineStr"/>
       <c r="F164" s="3">
@@ -10030,7 +10030,7 @@
         <v>472</v>
       </c>
       <c r="D165" s="3" t="n">
-        <v>2.75</v>
+        <v>2.4</v>
       </c>
       <c r="E165" s="3" t="inlineStr"/>
       <c r="F165" s="3">
@@ -10086,7 +10086,7 @@
         <v>472</v>
       </c>
       <c r="D166" s="3" t="n">
-        <v>2.21</v>
+        <v>2.02</v>
       </c>
       <c r="E166" s="3" t="inlineStr"/>
       <c r="F166" s="3">
@@ -10142,7 +10142,7 @@
         <v>472</v>
       </c>
       <c r="D167" s="3" t="n">
-        <v>2.04</v>
+        <v>1.91</v>
       </c>
       <c r="E167" s="3" t="inlineStr"/>
       <c r="F167" s="3">
@@ -10198,7 +10198,7 @@
         <v>465</v>
       </c>
       <c r="D168" s="3" t="n">
-        <v>18.38</v>
+        <v>19.49</v>
       </c>
       <c r="E168" s="3" t="inlineStr"/>
       <c r="F168" s="3">
@@ -10254,10 +10254,10 @@
         <v>40</v>
       </c>
       <c r="D169" s="3" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="E169" s="3" t="n">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="F169" s="3">
         <f>IF(B169="common", 4, IF(B169="uncommon", 3, IF(B169="rare", 0.73878, 1)))</f>
@@ -10312,7 +10312,7 @@
         <v>155</v>
       </c>
       <c r="D170" s="3" t="n">
-        <v>2.99</v>
+        <v>4.09</v>
       </c>
       <c r="E170" s="3" t="inlineStr"/>
       <c r="F170" s="3">
@@ -10368,7 +10368,7 @@
         <v>472</v>
       </c>
       <c r="D171" s="3" t="n">
-        <v>6.87</v>
+        <v>6.26</v>
       </c>
       <c r="E171" s="3" t="inlineStr"/>
       <c r="F171" s="3">
@@ -10424,7 +10424,7 @@
         <v>472</v>
       </c>
       <c r="D172" s="3" t="n">
-        <v>7.3</v>
+        <v>7.61</v>
       </c>
       <c r="E172" s="3" t="inlineStr"/>
       <c r="F172" s="3">
@@ -10480,10 +10480,10 @@
         <v>40</v>
       </c>
       <c r="D173" s="3" t="n">
-        <v>0.09</v>
+        <v>0.13</v>
       </c>
       <c r="E173" s="3" t="n">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="F173" s="3">
         <f>IF(B173="common", 4, IF(B173="uncommon", 3, IF(B173="rare", 0.73878, 1)))</f>
@@ -10538,7 +10538,7 @@
         <v>472</v>
       </c>
       <c r="D174" s="3" t="n">
-        <v>36.87</v>
+        <v>36.89</v>
       </c>
       <c r="E174" s="3" t="inlineStr"/>
       <c r="F174" s="3">
@@ -10594,7 +10594,7 @@
         <v>40</v>
       </c>
       <c r="D175" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E175" s="3" t="n">
         <v>0.1</v>
@@ -10652,7 +10652,7 @@
         <v>472</v>
       </c>
       <c r="D176" s="3" t="n">
-        <v>1.75</v>
+        <v>2.12</v>
       </c>
       <c r="E176" s="3" t="inlineStr"/>
       <c r="F176" s="3">
@@ -10711,7 +10711,7 @@
         <v>0.04</v>
       </c>
       <c r="E177" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F177" s="3">
         <f>IF(B177="common", 4, IF(B177="uncommon", 3, IF(B177="rare", 0.73878, 1)))</f>
@@ -10766,7 +10766,7 @@
         <v>472</v>
       </c>
       <c r="D178" s="3" t="n">
-        <v>3.25</v>
+        <v>3.37</v>
       </c>
       <c r="E178" s="3" t="inlineStr"/>
       <c r="F178" s="3">
@@ -10822,10 +10822,10 @@
         <v>16</v>
       </c>
       <c r="D179" s="3" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="E179" s="3" t="n">
-        <v>0.19</v>
+        <v>0.14</v>
       </c>
       <c r="F179" s="3">
         <f>IF(B179="common", 4, IF(B179="uncommon", 3, IF(B179="rare", 0.73878, 1)))</f>
@@ -10880,10 +10880,10 @@
         <v>16</v>
       </c>
       <c r="D180" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E180" s="3" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="F180" s="3">
         <f>IF(B180="common", 4, IF(B180="uncommon", 3, IF(B180="rare", 0.73878, 1)))</f>
@@ -10938,7 +10938,7 @@
         <v>472</v>
       </c>
       <c r="D181" s="3" t="n">
-        <v>1.88</v>
+        <v>1.48</v>
       </c>
       <c r="E181" s="3" t="inlineStr"/>
       <c r="F181" s="3">
@@ -10994,10 +10994,10 @@
         <v>16</v>
       </c>
       <c r="D182" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E182" s="3" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="F182" s="3">
         <f>IF(B182="common", 4, IF(B182="uncommon", 3, IF(B182="rare", 0.73878, 1)))</f>
@@ -11052,7 +11052,7 @@
         <v>472</v>
       </c>
       <c r="D183" s="3" t="n">
-        <v>9.630000000000001</v>
+        <v>10.06</v>
       </c>
       <c r="E183" s="3" t="inlineStr"/>
       <c r="F183" s="3">
@@ -11108,10 +11108,10 @@
         <v>40</v>
       </c>
       <c r="D184" s="3" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="E184" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F184" s="3">
         <f>IF(B184="common", 4, IF(B184="uncommon", 3, IF(B184="rare", 0.73878, 1)))</f>
@@ -11166,7 +11166,7 @@
         <v>472</v>
       </c>
       <c r="D185" s="3" t="n">
-        <v>12.77</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="E185" s="3" t="inlineStr"/>
       <c r="F185" s="3">
@@ -11222,10 +11222,10 @@
         <v>40</v>
       </c>
       <c r="D186" s="3" t="n">
-        <v>0.19</v>
+        <v>0.1</v>
       </c>
       <c r="E186" s="3" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="F186" s="3">
         <f>IF(B186="common", 4, IF(B186="uncommon", 3, IF(B186="rare", 0.73878, 1)))</f>
@@ -11280,7 +11280,7 @@
         <v>472</v>
       </c>
       <c r="D187" s="3" t="n">
-        <v>1.82</v>
+        <v>1.47</v>
       </c>
       <c r="E187" s="3" t="inlineStr"/>
       <c r="F187" s="3">
@@ -11336,10 +11336,10 @@
         <v>16</v>
       </c>
       <c r="D188" s="3" t="n">
-        <v>0.11</v>
+        <v>0.14</v>
       </c>
       <c r="E188" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F188" s="3">
         <f>IF(B188="common", 4, IF(B188="uncommon", 3, IF(B188="rare", 0.73878, 1)))</f>
@@ -11394,7 +11394,7 @@
         <v>472</v>
       </c>
       <c r="D189" s="3" t="n">
-        <v>2.67</v>
+        <v>2.17</v>
       </c>
       <c r="E189" s="3" t="inlineStr"/>
       <c r="F189" s="3">
@@ -11450,7 +11450,7 @@
         <v>472</v>
       </c>
       <c r="D190" s="3" t="n">
-        <v>7.81</v>
+        <v>8.01</v>
       </c>
       <c r="E190" s="3" t="inlineStr"/>
       <c r="F190" s="3">
@@ -11506,7 +11506,7 @@
         <v>472</v>
       </c>
       <c r="D191" s="3" t="n">
-        <v>3.65</v>
+        <v>4.72</v>
       </c>
       <c r="E191" s="3" t="inlineStr"/>
       <c r="F191" s="3">
@@ -11562,7 +11562,7 @@
         <v>472</v>
       </c>
       <c r="D192" s="3" t="n">
-        <v>7.53</v>
+        <v>7.68</v>
       </c>
       <c r="E192" s="3" t="inlineStr"/>
       <c r="F192" s="3">
@@ -11618,7 +11618,7 @@
         <v>472</v>
       </c>
       <c r="D193" s="3" t="n">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
       <c r="E193" s="3" t="inlineStr"/>
       <c r="F193" s="3">
@@ -11677,7 +11677,7 @@
         <v>0.05</v>
       </c>
       <c r="E194" s="3" t="n">
-        <v>0.13</v>
+        <v>0.17</v>
       </c>
       <c r="F194" s="3">
         <f>IF(B194="common", 4, IF(B194="uncommon", 3, IF(B194="rare", 0.73878, 1)))</f>
@@ -11732,10 +11732,10 @@
         <v>40</v>
       </c>
       <c r="D195" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E195" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="F195" s="3">
         <f>IF(B195="common", 4, IF(B195="uncommon", 3, IF(B195="rare", 0.73878, 1)))</f>
@@ -11790,7 +11790,7 @@
         <v>472</v>
       </c>
       <c r="D196" s="3" t="n">
-        <v>5.65</v>
+        <v>5.49</v>
       </c>
       <c r="E196" s="3" t="inlineStr"/>
       <c r="F196" s="3">
@@ -11846,7 +11846,7 @@
         <v>472</v>
       </c>
       <c r="D197" s="3" t="n">
-        <v>8.859999999999999</v>
+        <v>6.78</v>
       </c>
       <c r="E197" s="3" t="inlineStr"/>
       <c r="F197" s="3">
@@ -11902,7 +11902,7 @@
         <v>472</v>
       </c>
       <c r="D198" s="3" t="n">
-        <v>1.62</v>
+        <v>1.49</v>
       </c>
       <c r="E198" s="3" t="inlineStr"/>
       <c r="F198" s="3">
@@ -11958,7 +11958,7 @@
         <v>472</v>
       </c>
       <c r="D199" s="3" t="n">
-        <v>2.4</v>
+        <v>2.22</v>
       </c>
       <c r="E199" s="3" t="inlineStr"/>
       <c r="F199" s="3">
@@ -12014,7 +12014,7 @@
         <v>472</v>
       </c>
       <c r="D200" s="3" t="n">
-        <v>1.98</v>
+        <v>2.09</v>
       </c>
       <c r="E200" s="3" t="inlineStr"/>
       <c r="F200" s="3">
@@ -12070,7 +12070,7 @@
         <v>472</v>
       </c>
       <c r="D201" s="3" t="n">
-        <v>5.33</v>
+        <v>6.34</v>
       </c>
       <c r="E201" s="3" t="inlineStr"/>
       <c r="F201" s="3">
@@ -12126,7 +12126,7 @@
         <v>472</v>
       </c>
       <c r="D202" s="3" t="n">
-        <v>7.28</v>
+        <v>7.03</v>
       </c>
       <c r="E202" s="3" t="inlineStr"/>
       <c r="F202" s="3">
@@ -12182,7 +12182,7 @@
         <v>472</v>
       </c>
       <c r="D203" s="3" t="n">
-        <v>3.01</v>
+        <v>3.41</v>
       </c>
       <c r="E203" s="3" t="inlineStr"/>
       <c r="F203" s="3">
@@ -12238,7 +12238,7 @@
         <v>472</v>
       </c>
       <c r="D204" s="3" t="n">
-        <v>2.61</v>
+        <v>2.98</v>
       </c>
       <c r="E204" s="3" t="inlineStr"/>
       <c r="F204" s="3">
@@ -12294,7 +12294,7 @@
         <v>472</v>
       </c>
       <c r="D205" s="3" t="n">
-        <v>23.9</v>
+        <v>24.58</v>
       </c>
       <c r="E205" s="3" t="inlineStr"/>
       <c r="F205" s="3">
@@ -12350,7 +12350,7 @@
         <v>472</v>
       </c>
       <c r="D206" s="3" t="n">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="E206" s="3" t="inlineStr"/>
       <c r="F206" s="3">
@@ -12406,7 +12406,7 @@
         <v>472</v>
       </c>
       <c r="D207" s="3" t="n">
-        <v>3.68</v>
+        <v>4.55</v>
       </c>
       <c r="E207" s="3" t="inlineStr"/>
       <c r="F207" s="3">
@@ -12462,7 +12462,7 @@
         <v>63</v>
       </c>
       <c r="D208" s="3" t="n">
-        <v>0.68</v>
+        <v>0.82</v>
       </c>
       <c r="E208" s="3" t="inlineStr"/>
       <c r="F208" s="3">
@@ -12518,7 +12518,7 @@
         <v>155</v>
       </c>
       <c r="D209" s="3" t="n">
-        <v>1.22</v>
+        <v>1.13</v>
       </c>
       <c r="E209" s="3" t="inlineStr"/>
       <c r="F209" s="3">
@@ -12574,7 +12574,7 @@
         <v>472</v>
       </c>
       <c r="D210" s="3" t="n">
-        <v>4.7</v>
+        <v>5.27</v>
       </c>
       <c r="E210" s="3" t="inlineStr"/>
       <c r="F210" s="3">
@@ -12630,7 +12630,7 @@
         <v>472</v>
       </c>
       <c r="D211" s="3" t="n">
-        <v>3.82</v>
+        <v>3.88</v>
       </c>
       <c r="E211" s="3" t="inlineStr"/>
       <c r="F211" s="3">
@@ -12663,7 +12663,7 @@
         <v>0.05</v>
       </c>
       <c r="E212" s="3" t="n">
-        <v>0.21</v>
+        <v>0.14</v>
       </c>
       <c r="F212" s="3">
         <f>IF(B212="common", 4, IF(B212="uncommon", 3, IF(B212="rare", 0.73878, 1)))</f>
@@ -12698,10 +12698,10 @@
         <v>40</v>
       </c>
       <c r="D213" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E213" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F213" s="3">
         <f>IF(B213="common", 4, IF(B213="uncommon", 3, IF(B213="rare", 0.73878, 1)))</f>
@@ -12730,7 +12730,7 @@
         <v>472</v>
       </c>
       <c r="D214" s="3" t="n">
-        <v>10.22</v>
+        <v>10.52</v>
       </c>
       <c r="E214" s="3" t="inlineStr"/>
       <c r="F214" s="3">
@@ -12760,7 +12760,7 @@
         <v>472</v>
       </c>
       <c r="D215" s="3" t="n">
-        <v>4.6</v>
+        <v>4.8</v>
       </c>
       <c r="E215" s="3" t="inlineStr"/>
       <c r="F215" s="3">
@@ -12790,10 +12790,10 @@
         <v>25</v>
       </c>
       <c r="D216" s="3" t="n">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="E216" s="3" t="n">
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="F216" s="3">
         <f>IF(B216="common", 4, IF(B216="uncommon", 3, IF(B216="rare", 0.73878, 1)))</f>
@@ -12822,7 +12822,7 @@
         <v>472</v>
       </c>
       <c r="D217" s="3" t="n">
-        <v>2.26</v>
+        <v>2.63</v>
       </c>
       <c r="E217" s="3" t="inlineStr"/>
       <c r="F217" s="3">
@@ -12852,7 +12852,7 @@
         <v>372</v>
       </c>
       <c r="D218" s="3" t="n">
-        <v>5.38</v>
+        <v>4.99</v>
       </c>
       <c r="E218" s="3" t="inlineStr"/>
       <c r="F218" s="3">
@@ -12882,7 +12882,7 @@
         <v>472</v>
       </c>
       <c r="D219" s="3" t="n">
-        <v>3.94</v>
+        <v>3.88</v>
       </c>
       <c r="E219" s="3" t="inlineStr"/>
       <c r="F219" s="3">
@@ -12912,7 +12912,7 @@
         <v>472</v>
       </c>
       <c r="D220" s="3" t="n">
-        <v>6.35</v>
+        <v>6.1</v>
       </c>
       <c r="E220" s="3" t="inlineStr"/>
       <c r="F220" s="3">
@@ -12942,7 +12942,7 @@
         <v>472</v>
       </c>
       <c r="D221" s="3" t="n">
-        <v>3.98</v>
+        <v>3.24</v>
       </c>
       <c r="E221" s="3" t="inlineStr"/>
       <c r="F221" s="3">
@@ -12972,10 +12972,10 @@
         <v>40</v>
       </c>
       <c r="D222" s="3" t="n">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E222" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="F222" s="3">
         <f>IF(B222="common", 4, IF(B222="uncommon", 3, IF(B222="rare", 0.73878, 1)))</f>
@@ -13004,7 +13004,7 @@
         <v>472</v>
       </c>
       <c r="D223" s="3" t="n">
-        <v>2.54</v>
+        <v>2.74</v>
       </c>
       <c r="E223" s="3" t="inlineStr"/>
       <c r="F223" s="3">
@@ -13034,7 +13034,7 @@
         <v>63</v>
       </c>
       <c r="D224" s="3" t="n">
-        <v>0.5</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E224" s="3" t="inlineStr"/>
       <c r="F224" s="3">
@@ -13064,7 +13064,7 @@
         <v>155</v>
       </c>
       <c r="D225" s="3" t="n">
-        <v>1.35</v>
+        <v>0.93</v>
       </c>
       <c r="E225" s="3" t="inlineStr"/>
       <c r="F225" s="3">
@@ -13094,7 +13094,7 @@
         <v>472</v>
       </c>
       <c r="D226" s="3" t="n">
-        <v>2.69</v>
+        <v>2.87</v>
       </c>
       <c r="E226" s="3" t="inlineStr"/>
       <c r="F226" s="3">
@@ -13124,7 +13124,7 @@
         <v>472</v>
       </c>
       <c r="D227" s="3" t="n">
-        <v>1.73</v>
+        <v>1.91</v>
       </c>
       <c r="E227" s="3" t="inlineStr"/>
       <c r="F227" s="3">
@@ -13154,10 +13154,10 @@
         <v>25</v>
       </c>
       <c r="D228" s="3" t="n">
-        <v>0.16</v>
+        <v>0.11</v>
       </c>
       <c r="E228" s="3" t="n">
-        <v>0.43</v>
+        <v>0.35</v>
       </c>
       <c r="F228" s="3">
         <f>IF(B228="common", 4, IF(B228="uncommon", 3, IF(B228="rare", 0.73878, 1)))</f>
@@ -13186,10 +13186,10 @@
         <v>40</v>
       </c>
       <c r="D229" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E229" s="3" t="n">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="F229" s="3">
         <f>IF(B229="common", 4, IF(B229="uncommon", 3, IF(B229="rare", 0.73878, 1)))</f>
@@ -13218,7 +13218,7 @@
         <v>472</v>
       </c>
       <c r="D230" s="3" t="n">
-        <v>1.69</v>
+        <v>1.68</v>
       </c>
       <c r="E230" s="3" t="inlineStr"/>
       <c r="F230" s="3">
@@ -13248,7 +13248,7 @@
         <v>472</v>
       </c>
       <c r="D231" s="3" t="n">
-        <v>1.96</v>
+        <v>1.59</v>
       </c>
       <c r="E231" s="3" t="inlineStr"/>
       <c r="F231" s="3">
@@ -13278,7 +13278,7 @@
         <v>472</v>
       </c>
       <c r="D232" s="3" t="n">
-        <v>4.78</v>
+        <v>4.43</v>
       </c>
       <c r="E232" s="3" t="inlineStr"/>
       <c r="F232" s="3">
@@ -13308,7 +13308,7 @@
         <v>472</v>
       </c>
       <c r="D233" s="3" t="n">
-        <v>2.46</v>
+        <v>2.62</v>
       </c>
       <c r="E233" s="3" t="inlineStr"/>
       <c r="F233" s="3">
@@ -13338,7 +13338,7 @@
         <v>472</v>
       </c>
       <c r="D234" s="3" t="n">
-        <v>3.28</v>
+        <v>2.69</v>
       </c>
       <c r="E234" s="3" t="inlineStr"/>
       <c r="F234" s="3">
@@ -13368,7 +13368,7 @@
         <v>472</v>
       </c>
       <c r="D235" s="3" t="n">
-        <v>2.1</v>
+        <v>1.77</v>
       </c>
       <c r="E235" s="3" t="inlineStr"/>
       <c r="F235" s="3">
@@ -13398,10 +13398,10 @@
         <v>25</v>
       </c>
       <c r="D236" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E236" s="3" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="F236" s="3">
         <f>IF(B236="common", 4, IF(B236="uncommon", 3, IF(B236="rare", 0.73878, 1)))</f>
@@ -13430,7 +13430,7 @@
         <v>472</v>
       </c>
       <c r="D237" s="3" t="n">
-        <v>2.71</v>
+        <v>2.44</v>
       </c>
       <c r="E237" s="3" t="inlineStr"/>
       <c r="F237" s="3">
@@ -13460,7 +13460,7 @@
         <v>155</v>
       </c>
       <c r="D238" s="3" t="n">
-        <v>1.65</v>
+        <v>1.41</v>
       </c>
       <c r="E238" s="3" t="inlineStr"/>
       <c r="F238" s="3">
@@ -13490,7 +13490,7 @@
         <v>472</v>
       </c>
       <c r="D239" s="3" t="n">
-        <v>2.8</v>
+        <v>2.92</v>
       </c>
       <c r="E239" s="3" t="inlineStr"/>
       <c r="F239" s="3">
@@ -13520,7 +13520,7 @@
         <v>472</v>
       </c>
       <c r="D240" s="3" t="n">
-        <v>2.42</v>
+        <v>2.3</v>
       </c>
       <c r="E240" s="3" t="inlineStr"/>
       <c r="F240" s="3">
@@ -13550,7 +13550,7 @@
         <v>372</v>
       </c>
       <c r="D241" s="3" t="n">
-        <v>6.3</v>
+        <v>5.44</v>
       </c>
       <c r="E241" s="3" t="inlineStr"/>
       <c r="F241" s="3">
@@ -13580,10 +13580,10 @@
         <v>40</v>
       </c>
       <c r="D242" s="3" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E242" s="3" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="F242" s="3">
         <f>IF(B242="common", 4, IF(B242="uncommon", 3, IF(B242="rare", 0.73878, 1)))</f>
@@ -13612,7 +13612,7 @@
         <v>472</v>
       </c>
       <c r="D243" s="3" t="n">
-        <v>2.24</v>
+        <v>2.14</v>
       </c>
       <c r="E243" s="3" t="inlineStr"/>
       <c r="F243" s="3">
@@ -13642,7 +13642,7 @@
         <v>42</v>
       </c>
       <c r="D244" s="3" t="n">
-        <v>1.69</v>
+        <v>1.64</v>
       </c>
       <c r="E244" s="3" t="inlineStr"/>
       <c r="F244" s="3">
@@ -13672,10 +13672,10 @@
         <v>16</v>
       </c>
       <c r="D245" s="3" t="n">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="E245" s="3" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="F245" s="3">
         <f>IF(B245="common", 4, IF(B245="uncommon", 3, IF(B245="rare", 0.73878, 1)))</f>
@@ -13704,7 +13704,7 @@
         <v>472</v>
       </c>
       <c r="D246" s="3" t="n">
-        <v>2.47</v>
+        <v>2.71</v>
       </c>
       <c r="E246" s="3" t="inlineStr"/>
       <c r="F246" s="3">

</xml_diff>